<commit_message>
handled None value found error in views.py file
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="29">
   <si>
     <t>OrderDate</t>
   </si>
@@ -108,7 +108,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -148,7 +148,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -448,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -605,6 +605,123 @@
         <v>27</v>
       </c>
     </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="3">
+        <v>43831</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="3">
+        <v>43922</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="3">
+        <v>44013</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="3">
+        <v>44105</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="3">
+        <v>43842</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H11" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>